<commit_message>
Planning yard data wrangling
</commit_message>
<xml_diff>
--- a/yards_characteristics.xlsx
+++ b/yards_characteristics.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaliddell/Desktop/Jess_Honours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86FDDAA6-C65A-7641-82BA-6F2885A0FB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E8ACBA7-E946-2E4C-981E-E4CFE3165498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{9FE436D3-004D-E642-874C-9950AD24A8AF}"/>
+    <workbookView xWindow="12420" yWindow="740" windowWidth="16980" windowHeight="16880" xr2:uid="{9FE436D3-004D-E642-874C-9950AD24A8AF}"/>
   </bookViews>
   <sheets>
-    <sheet name="migratory" sheetId="1" r:id="rId1"/>
-    <sheet name="breeding" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,23 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>yard</t>
   </si>
   <si>
-    <t>centroid</t>
-  </si>
-  <si>
     <t>num_trees</t>
   </si>
   <si>
     <t>area</t>
   </si>
   <si>
-    <t>bird_SR</t>
-  </si>
-  <si>
     <t>tree_density</t>
   </si>
   <si>
@@ -130,6 +123,33 @@
   </si>
   <si>
     <t>fruit_tree</t>
+  </si>
+  <si>
+    <t>centroid_long</t>
+  </si>
+  <si>
+    <t>centroid_lat</t>
+  </si>
+  <si>
+    <t>SR_mig_24</t>
+  </si>
+  <si>
+    <t>SR_mig_25</t>
+  </si>
+  <si>
+    <t>SR_breed_24</t>
+  </si>
+  <si>
+    <t>SR_breed_25</t>
+  </si>
+  <si>
+    <t>SR_breed_tot</t>
+  </si>
+  <si>
+    <t>SR_mig_tot</t>
+  </si>
+  <si>
+    <t>SR_tot</t>
   </si>
 </sst>
 </file>
@@ -501,315 +521,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43097FE8-052A-C849-8842-6C21270B80EE}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="5" width="10.1640625" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="10.5" customWidth="1"/>
+    <col min="12" max="13" width="10.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B2">
+        <v>45.455219999999997</v>
+      </c>
+      <c r="C2">
+        <v>-73.644260000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B3">
+        <v>45.456110000000002</v>
+      </c>
+      <c r="C3">
+        <v>-73.644670000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2901013-2874-6247-BAC3-4F139BD35E2E}">
-  <dimension ref="A1:J22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
-    <col min="9" max="9" width="10.5" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" customWidth="1"/>
-    <col min="13" max="13" width="13.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>